<commit_message>
updated next weeks tasks
</commit_message>
<xml_diff>
--- a/Dashboards/milestone 5 Dashboard.xlsx
+++ b/Dashboards/milestone 5 Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanjager/Desktop/the-project-project-ricky/Dashboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05ACB51-3DCB-F64C-811D-079953A5DCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A23F17C-BE85-6849-A0C5-349124A54CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +144,20 @@
       <name val="Century Gothic"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -195,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -313,6 +327,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -326,7 +419,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -341,16 +434,10 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -368,21 +455,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="9" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -397,34 +469,16 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -438,6 +492,65 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2005,16 +2118,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>625231</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2200031</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>226024</xdr:rowOff>
+      <xdr:rowOff>276824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>3223846</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2258646</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>545124</xdr:rowOff>
+      <xdr:rowOff>595924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2042,7 +2155,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
+      <xdr:colOff>2717800</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>419100</xdr:rowOff>
     </xdr:from>
@@ -2065,8 +2178,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24587200" y="8445500"/>
-          <a:ext cx="13462000" cy="3009900"/>
+          <a:off x="26873200" y="8445500"/>
+          <a:ext cx="11176000" cy="3009900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2107,7 +2220,7 @@
               </a:solidFill>
               <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>The Process: The</a:t>
+            <a:t>The</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="3500" b="1" baseline="0">
@@ -10417,8 +10530,8 @@
       <xdr:rowOff>105834</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2857501</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>571500</xdr:rowOff>
     </xdr:to>
@@ -10435,8 +10548,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17371321" y="8917680"/>
-          <a:ext cx="2582334" cy="1442589"/>
+          <a:off x="579967" y="8970434"/>
+          <a:ext cx="2569634" cy="1456266"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -10605,15 +10718,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2844800</xdr:colOff>
+      <xdr:colOff>1625600</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>296333</xdr:rowOff>
+      <xdr:rowOff>245533</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2696308</xdr:colOff>
+      <xdr:colOff>1477108</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1172308</xdr:rowOff>
+      <xdr:rowOff>1121508</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -10628,8 +10741,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3137877" y="10085102"/>
-          <a:ext cx="2704123" cy="1501206"/>
+          <a:off x="1930400" y="10100733"/>
+          <a:ext cx="2696308" cy="1510975"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -10783,6 +10896,391 @@
               <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t> started quiz to class</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1244600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>613508</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12375</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="Snip Single Corner Rectangle 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1B0338E-A93A-7A49-A41D-438218BD8D6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4394200" y="8991600"/>
+          <a:ext cx="2696308" cy="1510975"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Style</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> some pages</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1350108</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1180775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Snip Single Corner Rectangle 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5F57444-E4D5-F14C-BB12-E2458C7A56F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="10160000"/>
+          <a:ext cx="2696308" cy="1510975"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Add</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> User security to the pages</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1800">
             <a:solidFill>
@@ -11143,22 +11641,22 @@
   </sheetPr>
   <dimension ref="B1:P15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" customWidth="1"/>
-    <col min="3" max="3" width="37.5" style="24" customWidth="1"/>
-    <col min="4" max="4" width="6" style="37" customWidth="1"/>
+    <col min="3" max="3" width="37.5" style="17" customWidth="1"/>
+    <col min="4" max="4" width="6" style="25" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="47.5" customWidth="1"/>
     <col min="7" max="7" width="40" customWidth="1"/>
     <col min="8" max="8" width="35.6640625" customWidth="1"/>
-    <col min="9" max="9" width="4" style="29" customWidth="1"/>
+    <col min="9" max="9" width="4" style="21" customWidth="1"/>
     <col min="10" max="11" width="45.83203125" customWidth="1"/>
     <col min="12" max="12" width="47" customWidth="1"/>
     <col min="13" max="13" width="3.1640625" customWidth="1"/>
@@ -11169,160 +11667,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="34"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="2:16" ht="43" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="23"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="2:16" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="31" t="s">
+      <c r="C3" s="43"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15" t="s">
+      <c r="I3" s="12"/>
+      <c r="J3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="47" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:16" s="14" customFormat="1" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="10"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="32"/>
+    <row r="4" spans="2:16" s="12" customFormat="1" ht="239" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="49"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="53"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="6"/>
-      <c r="N4" s="4"/>
+      <c r="L4" s="49"/>
+      <c r="N4" s="53"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="6"/>
+      <c r="P4" s="49"/>
     </row>
     <row r="5" spans="2:16" s="1" customFormat="1" ht="265" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="11"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="51"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="51"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="51"/>
     </row>
     <row r="6" spans="2:16" s="1" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C6" s="22"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="22"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="15"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="J7" s="38" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="27"/>
+      <c r="J7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
     </row>
     <row r="8" spans="2:16" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="41"/>
-      <c r="C8" s="42"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="36"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="29"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
     </row>
     <row r="9" spans="2:16" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="31"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="10" spans="2:16" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="43"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="28"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="31"/>
       <c r="I10"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
     </row>
     <row r="11" spans="2:16" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="45"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="26"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="33"/>
       <c r="I11"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
     </row>
     <row r="12" spans="2:16" ht="287" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
       <c r="I12"/>
     </row>
     <row r="13" spans="2:16" ht="44" customHeight="1" x14ac:dyDescent="0.2">
@@ -11366,7 +11876,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20"/>
+      <c r="A2" s="13"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Final report md created
</commit_message>
<xml_diff>
--- a/Dashboards/milestone 5 Dashboard.xlsx
+++ b/Dashboards/milestone 5 Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanjager/Desktop/the-project-project-ricky/Dashboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A23F17C-BE85-6849-A0C5-349124A54CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2E90F9-8270-A840-9626-CDE9CA4C11D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11641,9 +11641,9 @@
   </sheetPr>
   <dimension ref="B1:P15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="50" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11864,14 +11864,15 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="168" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>